<commit_message>
Test case 2 added
</commit_message>
<xml_diff>
--- a/Requirements and test cases.xlsx
+++ b/Requirements and test cases.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -70,10 +70,10 @@
     <t>Household budget</t>
   </si>
   <si>
-    <t>After logging in, I want to be redirected to my account home page</t>
-  </si>
-  <si>
-    <t>On the home page of the account there is a greeting "Witaj [user name]", and underneath there are options, one next to the other: "Wydatki", "Przychody", "Bilans", "Archiwum" and "Lista zakupów". After clicking on each of them, you will be redirected to separate, appropriate pages with the option of returning to the account home page by pressing the "Strona główna" link in the upper left corner.</t>
+    <t>After logging in I want to be redirected to my account home page</t>
+  </si>
+  <si>
+    <t>On the home page of the account there is a greeting "Witaj [user name]", and below there are options, one next to another: "Wydatki", "Przychody", "Bilans", "Archiwum" and "Lista zakupów". After clicking on each of them, you will be redirected to separate, appropriate pages with the option of returning to the account home page by pressing the "Strona główna" link in the upper left corner.</t>
   </si>
   <si>
     <t>Log out from the system</t>
@@ -162,6 +162,76 @@
   </si>
   <si>
     <t>User is logged in properly</t>
+  </si>
+  <si>
+    <t>Access to household budget funcionalities</t>
+  </si>
+  <si>
+    <t>The ability to manage own household budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is logged in correctly
+2. [user name] is known </t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Check if on the home page of the account there is greeting  "Witaj [user name]"</t>
+  </si>
+  <si>
+    <t>There is greeting "Witaj [user name]"</t>
+  </si>
+  <si>
+    <t>Check if below the greeting there are options, one next to the another: "Wydatki", "Przychody", "Bilans", "Archiwum" and "Lista zakupów"</t>
+  </si>
+  <si>
+    <t>All option are available</t>
+  </si>
+  <si>
+    <t>Click in "Wydatki"</t>
+  </si>
+  <si>
+    <t>User is redirected successfully to expenses page</t>
+  </si>
+  <si>
+    <t>Check if there is "Strona główna" link in upper left corner</t>
+  </si>
+  <si>
+    <t>"Strona główna" link is available in upper left corner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click in "Strona główna" link </t>
+  </si>
+  <si>
+    <t>User is redirected successfully to the home page of the account</t>
+  </si>
+  <si>
+    <t>Click in "Przychody"</t>
+  </si>
+  <si>
+    <t>User is redirected successfully to incomes page</t>
+  </si>
+  <si>
+    <t>Click in "Bilans"</t>
+  </si>
+  <si>
+    <t>User is redirected successfully to balance page</t>
+  </si>
+  <si>
+    <t>Click in "Archiwum"</t>
+  </si>
+  <si>
+    <t>User is redirected successfully to archives page</t>
+  </si>
+  <si>
+    <t>Click in "Lista zakupów"</t>
+  </si>
+  <si>
+    <t>User is redirected successfully to shopping list page</t>
   </si>
 </sst>
 </file>
@@ -273,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -346,7 +416,7 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -366,6 +436,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
@@ -1250,7 +1323,9 @@
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="33"/>
+      <c r="D3" s="21" t="s">
+        <v>48</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
@@ -1258,7 +1333,9 @@
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5">
@@ -1266,7 +1343,9 @@
         <v>2</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6">
@@ -1274,7 +1353,9 @@
         <v>3</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7">
@@ -1282,7 +1363,9 @@
         <v>4</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8">
@@ -1298,170 +1381,234 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="7">
+      <c r="B11" s="26">
         <v>1.0</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
+      <c r="C11" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="30"/>
     </row>
     <row r="12">
-      <c r="B12" s="7">
+      <c r="B12" s="26">
         <v>2.0</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
+      <c r="C12" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="30"/>
     </row>
     <row r="13">
-      <c r="B13" s="7">
+      <c r="B13" s="26">
         <v>3.0</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
+      <c r="C13" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="30"/>
     </row>
     <row r="14">
-      <c r="B14" s="7">
+      <c r="B14" s="26">
         <v>4.0</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="30"/>
     </row>
     <row r="15">
-      <c r="B15" s="7">
+      <c r="B15" s="26">
         <v>5.0</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
+      <c r="C15" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="30"/>
     </row>
     <row r="16">
-      <c r="B16" s="7">
+      <c r="B16" s="26">
         <v>6.0</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
+      <c r="C16" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="30"/>
     </row>
     <row r="17">
-      <c r="B17" s="7">
+      <c r="B17" s="26">
         <v>7.0</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
+      <c r="C17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="30"/>
     </row>
     <row r="18">
-      <c r="B18" s="7">
+      <c r="B18" s="26">
         <v>8.0</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
+      <c r="C18" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="30"/>
     </row>
     <row r="19">
-      <c r="B19" s="7">
+      <c r="B19" s="26">
         <v>9.0</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
+      <c r="C19" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="30"/>
     </row>
     <row r="20">
-      <c r="B20" s="7">
+      <c r="B20" s="26">
         <v>10.0</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
+      <c r="C20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="30"/>
     </row>
     <row r="21">
-      <c r="B21" s="7">
+      <c r="B21" s="26">
         <v>11.0</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
+      <c r="C21" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="30"/>
     </row>
     <row r="22">
-      <c r="B22" s="7">
+      <c r="B22" s="26">
         <v>12.0</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
+      <c r="C22" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="30"/>
     </row>
     <row r="23">
-      <c r="B23" s="7">
+      <c r="B23" s="26">
         <v>13.0</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
+      <c r="C23" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="30"/>
     </row>
     <row r="24">
-      <c r="B24" s="7">
+      <c r="B24" s="26">
         <v>14.0</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
+      <c r="C24" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="30"/>
     </row>
     <row r="25">
-      <c r="B25" s="7">
+      <c r="B25" s="26">
         <v>15.0</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
+      <c r="C25" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="30"/>
     </row>
     <row r="26">
-      <c r="B26" s="7">
+      <c r="B26" s="26">
         <v>16.0</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
+      <c r="C26" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="30"/>
     </row>
     <row r="27">
-      <c r="B27" s="7">
+      <c r="B27" s="26">
         <v>17.0</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
+      <c r="C27" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="30"/>
     </row>
     <row r="28">
-      <c r="B28" s="7">
-        <v>18.0</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
     </row>
     <row r="29">
-      <c r="B29" s="7">
-        <v>19.0</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1500,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
@@ -1750,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
@@ -2000,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4">

</xml_diff>